<commit_message>
Jun 11, 2024, 12:01 AM
</commit_message>
<xml_diff>
--- a/Main/static/CSVs/PC_Features.xlsx
+++ b/Main/static/CSVs/PC_Features.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\CS50-FinalProject\Main\static\CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4196C3-E1F9-4DE9-A371-FD681C32C5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D505DDBB-5820-484D-80C5-B189CD062508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14205" windowHeight="15585" activeTab="2" xr2:uid="{B488902C-D55E-47C3-8D97-FFB9C3833CE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B488902C-D55E-47C3-8D97-FFB9C3833CE3}"/>
   </bookViews>
   <sheets>
     <sheet name="pc_feature_list" sheetId="4" r:id="rId1"/>
-    <sheet name="individual_pc_features" sheetId="5" r:id="rId2"/>
-    <sheet name="Fighter_level_up" sheetId="6" r:id="rId3"/>
+    <sheet name="Fighter_level_up pseudo-code" sheetId="6" r:id="rId2"/>
+    <sheet name="individual_pc_features" sheetId="5" r:id="rId3"/>
     <sheet name="Metadata" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Fighter</t>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t>Python scripts calls AbilityScoreImprovement function</t>
+  </si>
+  <si>
+    <t>Improved Critical</t>
+  </si>
+  <si>
+    <t>Beginning when you choose this archetype at 3rd level, your weapon attacks score a critical hit on a roll of 19 or 20.</t>
+  </si>
+  <si>
+    <t>Remember that you can't make this entirely in SQL and sooner or later python will have to add stuff</t>
   </si>
 </sst>
 </file>
@@ -536,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DF8C6D-E654-4DC1-9038-77E4A221C97E}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,12 +697,97 @@
         <v>42</v>
       </c>
     </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DB3EFC-5FF5-4CFB-A06D-5DF2DAB400D5}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="22" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FF23EE-BF78-4EE3-8DFD-4F74F9CD8774}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -722,78 +816,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DB3EFC-5FF5-4CFB-A06D-5DF2DAB400D5}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="22" width="10.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Jun 11, 2024, 12:00 PM
</commit_message>
<xml_diff>
--- a/Main/static/CSVs/PC_Features.xlsx
+++ b/Main/static/CSVs/PC_Features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\CS50-FinalProject\Main\static\CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D505DDBB-5820-484D-80C5-B189CD062508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C380D73-5E50-4EC5-B2CB-22F03A7E61BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B488902C-D55E-47C3-8D97-FFB9C3833CE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B488902C-D55E-47C3-8D97-FFB9C3833CE3}"/>
   </bookViews>
   <sheets>
     <sheet name="pc_feature_list" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Fighter</t>
   </si>
@@ -153,12 +153,6 @@
     <t>The archetypal Champion focuses on the development of raw physical power honed to deadly perfection. Those who model themselves on this archetype combine rigorous training with physical excellence to deal devastating blows.</t>
   </si>
   <si>
-    <t>Tactician Fighter</t>
-  </si>
-  <si>
-    <t>The tactician focuses viewing the whole battlefield instead of just one foe. They looking to both direct allies towards unexpected advantages, as well to keep them from serious harm.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Python script offers choice of Archery, Defense, Dueling, GWF, Protection, TWF, and also adds Second Wind </t>
   </si>
   <si>
@@ -178,6 +172,21 @@
   </si>
   <si>
     <t>Remember that you can't make this entirely in SQL and sooner or later python will have to add stuff</t>
+  </si>
+  <si>
+    <t>Guardian</t>
+  </si>
+  <si>
+    <t>The guardian is a defensive fighter, focused on keeping their allies safe from harm, often putting themselves in the path of an attack meant for an ally.</t>
+  </si>
+  <si>
+    <t>Guardian Fighting Style</t>
+  </si>
+  <si>
+    <t>You gain the Protection fighting style if you do not already have it, or another fighting style of your choice if you do.</t>
+  </si>
+  <si>
+    <t>Guardian's Protection</t>
   </si>
 </sst>
 </file>
@@ -545,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DF8C6D-E654-4DC1-9038-77E4A221C97E}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,18 +700,31 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -714,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DB3EFC-5FF5-4CFB-A06D-5DF2DAB400D5}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -740,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -751,7 +773,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -762,7 +784,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -773,12 +795,12 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>